<commit_message>
Fix vocation judgement again, finally fixed
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1083,9 +1083,9 @@
           <t>正常</t>
         </is>
       </c>
-      <c r="N6" s="4" t="inlineStr">
-        <is>
-          <t>上班正常,下班早退252分钟,</t>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>正常</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
@@ -3328,9 +3328,9 @@
           <t>正常</t>
         </is>
       </c>
-      <c r="K26" s="4" t="inlineStr">
-        <is>
-          <t>上班正常,下班早退111分钟,</t>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>正常</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
@@ -4593,7 +4593,7 @@
       </c>
       <c r="O37" s="4" t="inlineStr">
         <is>
-          <t>上班正常,下班早退97分钟,</t>
+          <t>上班正常,下班早退7分钟,</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -4684,9 +4684,9 @@
           <t>正常</t>
         </is>
       </c>
-      <c r="K38" s="4" t="inlineStr">
-        <is>
-          <t>上班正常,下班早退27分钟,</t>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>正常</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
@@ -4699,9 +4699,9 @@
           <t>正常</t>
         </is>
       </c>
-      <c r="N38" s="4" t="inlineStr">
-        <is>
-          <t>上班正常,下班早退30分钟,</t>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>正常</t>
         </is>
       </c>
       <c r="O38" t="inlineStr">
@@ -4709,9 +4709,9 @@
           <t>正常</t>
         </is>
       </c>
-      <c r="P38" s="4" t="inlineStr">
-        <is>
-          <t>上班正常,下班早退29分钟,</t>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>正常</t>
         </is>
       </c>
       <c r="Q38" t="inlineStr">
@@ -4772,9 +4772,9 @@
           <t>正常</t>
         </is>
       </c>
-      <c r="F39" s="4" t="inlineStr">
-        <is>
-          <t>上班正常,下班早退26分钟,</t>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>正常</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -4842,9 +4842,9 @@
           <t>上班迟到46分钟,下班早退167分钟,</t>
         </is>
       </c>
-      <c r="T39" s="4" t="inlineStr">
-        <is>
-          <t>上班正常,下班早退29分钟,</t>
+      <c r="T39" t="inlineStr">
+        <is>
+          <t>正常</t>
         </is>
       </c>
       <c r="U39" t="inlineStr">
@@ -4852,9 +4852,9 @@
           <t>正常</t>
         </is>
       </c>
-      <c r="V39" s="4" t="inlineStr">
-        <is>
-          <t>上班正常,下班早退190分钟,</t>
+      <c r="V39" t="inlineStr">
+        <is>
+          <t>正常</t>
         </is>
       </c>
       <c r="W39" t="inlineStr">
@@ -5424,7 +5424,7 @@
       </c>
       <c r="W44" s="4" t="inlineStr">
         <is>
-          <t>上班正常,下班早退215分钟,</t>
+          <t>上班正常,下班早退25分钟,</t>
         </is>
       </c>
     </row>
@@ -6615,9 +6615,9 @@
           <t>正常</t>
         </is>
       </c>
-      <c r="M55" s="4" t="inlineStr">
-        <is>
-          <t>上班正常,下班早退94分钟,</t>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>正常</t>
         </is>
       </c>
       <c r="N55" t="inlineStr">
@@ -7745,9 +7745,9 @@
           <t>正常</t>
         </is>
       </c>
-      <c r="M65" s="4" t="inlineStr">
-        <is>
-          <t>上班正常,下班早退212分钟,</t>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>正常</t>
         </is>
       </c>
       <c r="N65" t="inlineStr">
@@ -7770,9 +7770,9 @@
           <t>正常</t>
         </is>
       </c>
-      <c r="R65" s="4" t="inlineStr">
-        <is>
-          <t>上班正常,下班早退206分钟,</t>
+      <c r="R65" t="inlineStr">
+        <is>
+          <t>正常</t>
         </is>
       </c>
       <c r="S65" s="2" t="inlineStr">
@@ -8011,9 +8011,9 @@
           <t>正常</t>
         </is>
       </c>
-      <c r="U67" s="4" t="inlineStr">
-        <is>
-          <t>上班正常,下班早退218分钟,</t>
+      <c r="U67" t="inlineStr">
+        <is>
+          <t>正常</t>
         </is>
       </c>
       <c r="V67" t="inlineStr">
@@ -8448,9 +8448,9 @@
           <t>正常</t>
         </is>
       </c>
-      <c r="R71" s="4" t="inlineStr">
-        <is>
-          <t>上班正常,下班早退60分钟,</t>
+      <c r="R71" t="inlineStr">
+        <is>
+          <t>正常</t>
         </is>
       </c>
       <c r="S71" s="4" t="inlineStr">
@@ -8583,7 +8583,7 @@
       </c>
       <c r="V72" s="4" t="inlineStr">
         <is>
-          <t>上班正常,下班早退172分钟,</t>
+          <t>上班正常,下班早退112分钟,</t>
         </is>
       </c>
       <c r="W72" t="inlineStr">
@@ -9711,9 +9711,9 @@
           <t>正常</t>
         </is>
       </c>
-      <c r="V82" s="4" t="inlineStr">
-        <is>
-          <t>上班正常,下班早退279分钟,</t>
+      <c r="V82" t="inlineStr">
+        <is>
+          <t>正常</t>
         </is>
       </c>
       <c r="W82" t="inlineStr">
@@ -11064,7 +11064,7 @@
       </c>
       <c r="U94" s="2" t="inlineStr">
         <is>
-          <t>上班迟到2分钟,下班早退60分钟,</t>
+          <t>上班迟到2分钟,下班正常</t>
         </is>
       </c>
       <c r="V94" t="inlineStr">
@@ -11162,7 +11162,7 @@
       </c>
       <c r="R95" s="4" t="inlineStr">
         <is>
-          <t>上班正常,下班早退67分钟,</t>
+          <t>上班正常,下班早退7分钟,</t>
         </is>
       </c>
       <c r="S95" s="4" t="inlineStr">
@@ -12157,9 +12157,9 @@
           <t>正常</t>
         </is>
       </c>
-      <c r="N104" s="4" t="inlineStr">
-        <is>
-          <t>上班正常,下班早退215分钟,</t>
+      <c r="N104" t="inlineStr">
+        <is>
+          <t>正常</t>
         </is>
       </c>
       <c r="O104" t="inlineStr">
@@ -13648,7 +13648,7 @@
       </c>
       <c r="R117" s="4" t="inlineStr">
         <is>
-          <t>上班正常,下班早退60分钟,</t>
+          <t>上班正常,下班早退35分钟,</t>
         </is>
       </c>
       <c r="S117" s="2" t="inlineStr">
@@ -16699,7 +16699,7 @@
       </c>
       <c r="R144" s="2" t="inlineStr">
         <is>
-          <t>上班迟到1分钟,下班早退52分钟,</t>
+          <t>上班迟到1分钟,下班正常</t>
         </is>
       </c>
       <c r="S144" s="2" t="inlineStr">
@@ -21274,9 +21274,9 @@
           <t>正常</t>
         </is>
       </c>
-      <c r="R185" s="4" t="inlineStr">
-        <is>
-          <t>上班正常,下班早退60分钟,</t>
+      <c r="R185" t="inlineStr">
+        <is>
+          <t>正常</t>
         </is>
       </c>
       <c r="S185" s="2" t="inlineStr">
@@ -22645,9 +22645,9 @@
           <t>正常</t>
         </is>
       </c>
-      <c r="U197" s="4" t="inlineStr">
-        <is>
-          <t>上班正常,下班早退287分钟,</t>
+      <c r="U197" t="inlineStr">
+        <is>
+          <t>正常</t>
         </is>
       </c>
       <c r="V197" t="inlineStr">

</xml_diff>

<commit_message>
Fix mistakenly handling for overlapped absence leaves
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -4360,9 +4360,9 @@
           <t>正常</t>
         </is>
       </c>
-      <c r="N35" s="2" t="inlineStr">
-        <is>
-          <t>上班迟到27分钟,下班正常</t>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>正常</t>
         </is>
       </c>
       <c r="O35" t="inlineStr">
@@ -4468,9 +4468,9 @@
           <t>上班迟到653分钟,下班缺卡</t>
         </is>
       </c>
-      <c r="M36" s="2" t="inlineStr">
-        <is>
-          <t>上班迟到138分钟,下班正常</t>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>正常</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
@@ -11735,9 +11735,9 @@
           <t>上班正常,下班早退147分钟,</t>
         </is>
       </c>
-      <c r="T100" s="3" t="inlineStr">
-        <is>
-          <t>旷工</t>
+      <c r="T100" t="inlineStr">
+        <is>
+          <t>休假</t>
         </is>
       </c>
       <c r="U100" t="inlineStr">

</xml_diff>

<commit_message>
Merge the overlapped absence leave records first, then processing data.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -8581,9 +8581,9 @@
           <t>正常</t>
         </is>
       </c>
-      <c r="V72" s="4" t="inlineStr">
-        <is>
-          <t>上班正常,下班早退112分钟,</t>
+      <c r="V72" t="inlineStr">
+        <is>
+          <t>正常</t>
         </is>
       </c>
       <c r="W72" t="inlineStr">

</xml_diff>